<commit_message>
update Jan 23 2025
</commit_message>
<xml_diff>
--- a/Version_on_pcloud/Data_processing_notebooks/Data_processing_KS20-527/Notebook_Compiled_data/K20_Raman_averaged.xlsx
+++ b/Version_on_pcloud/Data_processing_notebooks/Data_processing_KS20-527/Notebook_Compiled_data/K20_Raman_averaged.xlsx
@@ -1711,7 +1711,7 @@
       <c r="DD2" t="inlineStr"/>
       <c r="DE2" t="inlineStr"/>
       <c r="DF2" t="n">
-        <v>0.004832970503648978</v>
+        <v>0.004832970503648979</v>
       </c>
       <c r="DG2" t="n">
         <v>0.0003687115304388325</v>
@@ -1755,7 +1755,7 @@
         <v>0.0001636821790030073</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.004832970503648978</v>
+        <v>0.004832970503648979</v>
       </c>
       <c r="DW2" t="n">
         <v>0.0003687115304388325</v>
@@ -1815,7 +1815,7 @@
         <v>70.50072994865353</v>
       </c>
       <c r="EP2" t="n">
-        <v>0.00323854315347735</v>
+        <v>0.003238543153477349</v>
       </c>
       <c r="EQ2" t="n">
         <v>0</v>
@@ -1848,7 +1848,7 @@
         <v>0.1277471358909658</v>
       </c>
       <c r="FK2" t="n">
-        <v>0.09796047447211081</v>
+        <v>0.09796047447211083</v>
       </c>
       <c r="FL2" t="n">
         <v>0.2586991369902635</v>
@@ -2314,10 +2314,10 @@
         <v>1.3893404978127</v>
       </c>
       <c r="EI3" t="n">
-        <v>0.01748610600565654</v>
+        <v>0.01748610600565653</v>
       </c>
       <c r="EJ3" t="n">
-        <v>0.04330182253267002</v>
+        <v>0.04330182253267001</v>
       </c>
       <c r="EK3" t="n">
         <v>0.002373694822749665</v>
@@ -2392,7 +2392,7 @@
         <v>0.01086755374164359</v>
       </c>
       <c r="FQ3" t="n">
-        <v>5.590195512312427e-06</v>
+        <v>5.590195512312428e-06</v>
       </c>
       <c r="FR3" t="n">
         <v>0</v>
@@ -2825,7 +2825,7 @@
         <v>0.0002171090930033541</v>
       </c>
       <c r="EB4" t="n">
-        <v>0.03076061906781654</v>
+        <v>0.03076061906781653</v>
       </c>
       <c r="EC4" t="n">
         <v>0.0001860388314832264</v>
@@ -2834,7 +2834,7 @@
         <v>45.31959509720662</v>
       </c>
       <c r="EE4" t="n">
-        <v>0.03076061906776445</v>
+        <v>0.03076061906776444</v>
       </c>
       <c r="EF4" t="n">
         <v>110.0439629918911</v>
@@ -3319,7 +3319,7 @@
         <v>0.002657140020052187</v>
       </c>
       <c r="DN5" t="n">
-        <v>0.009165151389911469</v>
+        <v>0.009165151389911471</v>
       </c>
       <c r="DO5" t="n">
         <v>0</v>
@@ -3357,7 +3357,7 @@
         <v>0.002657140020052187</v>
       </c>
       <c r="EB5" t="n">
-        <v>0.04363865180453827</v>
+        <v>0.04363865180453826</v>
       </c>
       <c r="EC5" t="n">
         <v>0.002003255814079039</v>
@@ -3366,7 +3366,7 @@
         <v>155.8449420730669</v>
       </c>
       <c r="EE5" t="n">
-        <v>0.04363865180453827</v>
+        <v>0.04363865180453826</v>
       </c>
       <c r="EF5" t="n">
         <v>432.9609650333171</v>
@@ -3381,10 +3381,10 @@
         <v>0.03909668415009844</v>
       </c>
       <c r="EJ5" t="n">
-        <v>0.01642036681494803</v>
+        <v>0.01642036681494804</v>
       </c>
       <c r="EK5" t="n">
-        <v>0.02427342317049297</v>
+        <v>0.02427342317049296</v>
       </c>
       <c r="EL5" t="n">
         <v>0.001984537762946304</v>
@@ -3833,7 +3833,7 @@
         <v>9.35129521204048e-07</v>
       </c>
       <c r="DJ6" t="n">
-        <v>0.007210467132182745</v>
+        <v>0.007210467132182746</v>
       </c>
       <c r="DK6" t="n">
         <v>0.0002304850791961425</v>
@@ -3862,7 +3862,7 @@
         <v>0.002857076527787342</v>
       </c>
       <c r="DU6" t="n">
-        <v>5.52022941336663e-05</v>
+        <v>5.520229413366629e-05</v>
       </c>
       <c r="DV6" t="n">
         <v>0.00368009754341232</v>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="ER6" t="n">
-        <v>0.07332998605063307</v>
+        <v>0.07332998605063305</v>
       </c>
       <c r="ES6" t="n">
         <v>0.009532076860937745</v>
@@ -3958,7 +3958,7 @@
         <v>1.983760221304842</v>
       </c>
       <c r="FE6" t="n">
-        <v>42.18958180234007</v>
+        <v>42.18958180234006</v>
       </c>
       <c r="FF6" t="n">
         <v>1.882053819896045</v>
@@ -3973,7 +3973,7 @@
         <v>0.0139454484470955</v>
       </c>
       <c r="FL6" t="n">
-        <v>0.06750483955959083</v>
+        <v>0.06750483955959084</v>
       </c>
       <c r="FM6" t="n">
         <v>0.0002145247470159356</v>
@@ -16079,7 +16079,7 @@
         <v>0.002179254883697967</v>
       </c>
       <c r="DN34" t="n">
-        <v>0.07544534445544122</v>
+        <v>0.07544534445544124</v>
       </c>
       <c r="DO34" t="n">
         <v>0</v>
@@ -16138,13 +16138,13 @@
         <v>0.7585899050411115</v>
       </c>
       <c r="EI34" t="n">
-        <v>0.03978111779819275</v>
+        <v>0.03978111779819276</v>
       </c>
       <c r="EJ34" t="n">
         <v>0.02235448469364748</v>
       </c>
       <c r="EK34" t="n">
-        <v>0.002801861622381327</v>
+        <v>0.002801861622381328</v>
       </c>
       <c r="EL34" t="n">
         <v>0.004613231536422408</v>
@@ -16156,7 +16156,7 @@
         <v>0.002766349453855479</v>
       </c>
       <c r="EO34" t="n">
-        <v>84.99778839562003</v>
+        <v>84.99778839562005</v>
       </c>
       <c r="EP34" t="n">
         <v>0.007754067145160279</v>
@@ -16210,7 +16210,7 @@
         <v>0.0239874842117029</v>
       </c>
       <c r="FM34" t="n">
-        <v>0.0003249345407530975</v>
+        <v>0.0003249345407530976</v>
       </c>
       <c r="FN34" t="n">
         <v>0.005837556812703111</v>
@@ -16615,7 +16615,7 @@
       <c r="DD35" t="inlineStr"/>
       <c r="DE35" t="inlineStr"/>
       <c r="DF35" t="n">
-        <v>0.007195608131690942</v>
+        <v>0.007195608131690943</v>
       </c>
       <c r="DG35" t="n">
         <v>0.01190453766005759</v>
@@ -16653,7 +16653,7 @@
       <c r="DR35" t="inlineStr"/>
       <c r="DS35" t="inlineStr"/>
       <c r="DT35" t="n">
-        <v>0.007195608131690942</v>
+        <v>0.007195608131690943</v>
       </c>
       <c r="DU35" t="n">
         <v>0.01190453766005759</v>
@@ -17223,7 +17223,7 @@
         <v>0.006568974226111232</v>
       </c>
       <c r="EF36" t="n">
-        <v>9.623457155447099</v>
+        <v>9.623457155447101</v>
       </c>
       <c r="EG36" t="n">
         <v>0.01708252116098879</v>
@@ -17685,7 +17685,7 @@
         <v>0.01895480443921532</v>
       </c>
       <c r="DL37" t="n">
-        <v>3.270235687701335e-06</v>
+        <v>3.270235687701336e-06</v>
       </c>
       <c r="DM37" t="n">
         <v>0.01900360475320047</v>
@@ -17747,7 +17747,7 @@
         <v>0.0594836868164027</v>
       </c>
       <c r="EH37" t="n">
-        <v>0.3571006005535773</v>
+        <v>0.3571006005535772</v>
       </c>
       <c r="EI37" t="n">
         <v>0.2933798310125425</v>

</xml_diff>